<commit_message>
Added Digikey part numbers to everything and put in how many I will order and what the volume prices are.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckillion\Documents\DipTrace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckillion\Documents\DipTrace\Projects\SDTx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="148">
   <si>
     <t>#</t>
   </si>
@@ -373,6 +373,96 @@
   </si>
   <si>
     <t>XC2062CT-ND</t>
+  </si>
+  <si>
+    <t>1276-1005-1-ND</t>
+  </si>
+  <si>
+    <t>Qty Ordered</t>
+  </si>
+  <si>
+    <t>Cost @ Qty</t>
+  </si>
+  <si>
+    <t>1276-2868-1-ND</t>
+  </si>
+  <si>
+    <t>490-10470-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1927-1-ND</t>
+  </si>
+  <si>
+    <t>1276-2087-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1034-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1085-1-ND</t>
+  </si>
+  <si>
+    <t>1276-2078-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1278-1-ND</t>
+  </si>
+  <si>
+    <t>1276-2184-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1135-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1018-1-ND</t>
+  </si>
+  <si>
+    <t>160-1434-1-ND</t>
+  </si>
+  <si>
+    <t>S9000-ND</t>
+  </si>
+  <si>
+    <t>535-11597-1-ND</t>
+  </si>
+  <si>
+    <t>311-100KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-40.2KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-7.68KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-150HRCT-ND</t>
+  </si>
+  <si>
+    <t>311-75.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-2.00KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-10.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-1.00KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-160HRCT-ND</t>
+  </si>
+  <si>
+    <t>311-100HRCT-ND</t>
+  </si>
+  <si>
+    <t>311-51.0HRCT-ND</t>
+  </si>
+  <si>
+    <t>311-75.0HRCT-ND</t>
+  </si>
+  <si>
+    <t>311-4.70KHRCT-ND</t>
   </si>
 </sst>
 </file>
@@ -382,7 +472,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,10 +608,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -866,15 +965,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1233,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G43" sqref="G2:G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,12 +1349,14 @@
     <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="12.42578125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="12.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.140625" style="2"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1271,14 +1375,20 @@
       <c r="F1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1294,15 +1404,24 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="F2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H2" s="2">
         <f>D2*G2</f>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1">
+        <v>500</v>
+      </c>
+      <c r="J2" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1318,15 +1437,24 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="F3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H3" s="2">
         <f t="shared" ref="H3:H43" si="0">D3*G3</f>
         <v>0.06</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.13239999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1342,15 +1470,24 @@
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="F4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H4" s="2">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2">
+        <v>6.9599999999999995E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1366,15 +1503,24 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I5" s="1">
+        <v>25</v>
+      </c>
+      <c r="J5" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1390,15 +1536,24 @@
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H6" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I6" s="1">
+        <v>25</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5.2400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1414,15 +1569,24 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H7" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I7" s="1">
+        <v>25</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.5599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1438,15 +1602,24 @@
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="F8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H8" s="2">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="1">
+        <v>25</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2.9600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1462,15 +1635,24 @@
       <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I9" s="1">
+        <v>25</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.44E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1486,15 +1668,24 @@
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="F10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H10" s="2">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1">
+        <v>25</v>
+      </c>
+      <c r="J10" s="2">
+        <v>8.8000000000000005E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1510,15 +1701,24 @@
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H11" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I11" s="1">
+        <v>25</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1.1599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1534,15 +1734,24 @@
       <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="F12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H12" s="2">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1">
+        <v>50</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1.04E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1558,15 +1767,24 @@
       <c r="E13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="F13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H13" s="2">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="1">
+        <v>50</v>
+      </c>
+      <c r="J13" s="2">
+        <v>9.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1582,15 +1800,24 @@
       <c r="E14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="3">
+      <c r="F14" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="2">
         <v>0.1</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="1">
+        <v>50</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.1348</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1606,18 +1833,24 @@
       <c r="E15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <f t="shared" si="0"/>
         <v>1.1299999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="1">
+        <v>4</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1636,15 +1869,21 @@
       <c r="F16" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <v>1.89</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <f>D16*G16</f>
         <v>1.89</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1">
+        <v>4</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1660,15 +1899,24 @@
       <c r="E17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="3">
+      <c r="F17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G17" s="2">
         <v>0.1</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1">
+        <v>10</v>
+      </c>
+      <c r="J17" s="2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1687,15 +1935,21 @@
       <c r="F18" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <v>0.4</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1">
+        <v>4</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1714,15 +1968,21 @@
       <c r="F19" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <v>2.15</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <f t="shared" si="0"/>
         <v>2.15</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1">
+        <v>4</v>
+      </c>
+      <c r="J19" s="2">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1741,15 +2001,21 @@
       <c r="F20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>0.4</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1">
+        <v>4</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1765,15 +2031,24 @@
       <c r="E21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="3">
+      <c r="F21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" s="2">
         <v>0.05</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1">
+        <v>25</v>
+      </c>
+      <c r="J21" s="2">
+        <v>7.6399999999999996E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1789,15 +2064,24 @@
       <c r="E22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H22" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I22" s="1">
+        <v>10</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1813,15 +2097,24 @@
       <c r="E23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H23" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I23" s="1">
+        <v>10</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1837,15 +2130,24 @@
       <c r="E24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H24" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I24" s="1">
+        <v>10</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1861,15 +2163,24 @@
       <c r="E25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H25" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I25" s="1">
+        <v>10</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1885,15 +2196,24 @@
       <c r="E26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G26" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H26" s="3">
+      <c r="F26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H26" s="2">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1">
+        <v>25</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1909,15 +2229,24 @@
       <c r="E27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H27" s="3">
+      <c r="F27" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H27" s="2">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="1">
+        <v>25</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1933,15 +2262,24 @@
       <c r="E28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G28" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H28" s="3">
+      <c r="F28" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H28" s="2">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="1">
+        <v>25</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1957,15 +2295,24 @@
       <c r="E29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H29" s="3">
+      <c r="F29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H29" s="2">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="1">
+        <v>25</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1981,15 +2328,24 @@
       <c r="E30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H30" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I30" s="1">
+        <v>10</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2005,15 +2361,24 @@
       <c r="E31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H31" s="3">
+      <c r="F31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H31" s="2">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1">
+        <v>100</v>
+      </c>
+      <c r="J31" s="2">
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2029,15 +2394,24 @@
       <c r="E32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H32" s="3">
+      <c r="F32" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H32" s="2">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1">
+        <v>25</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2053,15 +2427,24 @@
       <c r="E33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H33" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I33" s="1">
+        <v>10</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2077,15 +2460,24 @@
       <c r="E34" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G34" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="H34" s="3">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I34" s="1">
+        <v>10</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2104,15 +2496,21 @@
       <c r="F35" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="2">
         <v>1.25</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="2">
         <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1">
+        <v>12</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1.2010000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2131,15 +2529,21 @@
       <c r="F36" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="2">
         <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="1">
+        <v>10</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2158,15 +2562,15 @@
       <c r="F37" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="2">
         <v>18.45</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="2">
         <f t="shared" si="0"/>
         <v>18.45</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2185,15 +2589,21 @@
       <c r="F38" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="2">
         <v>10.58</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="2">
         <f t="shared" si="0"/>
         <v>10.58</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="1">
+        <v>4</v>
+      </c>
+      <c r="J38" s="2">
+        <v>10.58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2212,15 +2622,21 @@
       <c r="F39" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="2">
         <v>0.92</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="2">
         <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1">
+        <v>5</v>
+      </c>
+      <c r="J39" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2239,15 +2655,21 @@
       <c r="F40" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="2">
         <v>0.46</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="2">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1">
+        <v>10</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0.373</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2266,15 +2688,15 @@
       <c r="F41" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="2">
         <v>16.899999999999999</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="2">
         <f t="shared" si="0"/>
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2287,12 +2709,12 @@
       <c r="E42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2311,25 +2733,34 @@
       <c r="F43" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="2">
         <v>2.71</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="2">
         <f t="shared" si="0"/>
         <v>2.71</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1">
+        <v>5</v>
+      </c>
+      <c r="J43" s="2">
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D44" s="1">
         <v>109</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="2">
         <f>SUM(H2:H43)</f>
         <v>62.779999999999994</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J1" r:id="rId1" display="Cost@Qty"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added GALI-3+ part number and costs to BOM.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="151">
   <si>
     <t>#</t>
   </si>
@@ -463,6 +463,15 @@
   </si>
   <si>
     <t>311-4.70KHRCT-ND</t>
+  </si>
+  <si>
+    <t>Order Cost</t>
+  </si>
+  <si>
+    <t>Amplifier</t>
+  </si>
+  <si>
+    <t>MiniCircuits GALI-3+</t>
   </si>
 </sst>
 </file>
@@ -965,7 +974,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -977,6 +986,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1335,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G43" sqref="G2:G43"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,7 +1368,7 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1387,8 +1399,11 @@
       <c r="J1" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1420,8 +1435,12 @@
       <c r="J2" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="5">
+        <f>I2*J2</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1453,8 +1472,12 @@
       <c r="J3" s="2">
         <v>0.13239999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="5">
+        <f t="shared" ref="K3:K43" si="1">I3*J3</f>
+        <v>3.3099999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1486,8 +1509,12 @@
       <c r="J4" s="2">
         <v>6.9599999999999995E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7399999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1519,8 +1546,12 @@
       <c r="J5" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="5">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1552,8 +1583,12 @@
       <c r="J6" s="2">
         <v>5.2400000000000002E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="5">
+        <f t="shared" si="1"/>
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1585,8 +1620,12 @@
       <c r="J7" s="2">
         <v>1.5599999999999999E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.38999999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1618,8 +1657,12 @@
       <c r="J8" s="2">
         <v>2.9600000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="5">
+        <f t="shared" si="1"/>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1651,8 +1694,12 @@
       <c r="J9" s="2">
         <v>1.44E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="5">
+        <f t="shared" si="1"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1684,8 +1731,12 @@
       <c r="J10" s="2">
         <v>8.8000000000000005E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="5">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1717,8 +1768,12 @@
       <c r="J11" s="2">
         <v>1.1599999999999999E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1750,8 +1805,12 @@
       <c r="J12" s="2">
         <v>1.04E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="5">
+        <f t="shared" si="1"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1783,8 +1842,12 @@
       <c r="J13" s="2">
         <v>9.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="5">
+        <f t="shared" si="1"/>
+        <v>0.45999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1816,8 +1879,12 @@
       <c r="J14" s="2">
         <v>0.1348</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="5">
+        <f t="shared" si="1"/>
+        <v>6.74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1849,8 +1916,12 @@
       <c r="J15" s="2">
         <v>1.1299999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="5">
+        <f t="shared" si="1"/>
+        <v>4.5199999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1882,8 +1953,12 @@
       <c r="J16" s="2">
         <v>1.89</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="5">
+        <f t="shared" si="1"/>
+        <v>7.56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1915,8 +1990,12 @@
       <c r="J17" s="2">
         <v>7.6999999999999999E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="5">
+        <f t="shared" si="1"/>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1948,8 +2027,12 @@
       <c r="J18" s="2">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="5">
+        <f t="shared" si="1"/>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1981,8 +2064,12 @@
       <c r="J19" s="2">
         <v>2.15</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="5">
+        <f t="shared" si="1"/>
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2012,10 +2099,14 @@
         <v>4</v>
       </c>
       <c r="J20" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2047,8 +2138,12 @@
       <c r="J21" s="2">
         <v>7.6399999999999996E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="5">
+        <f t="shared" si="1"/>
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2080,8 +2175,12 @@
       <c r="J22" s="2">
         <v>1.4E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="5">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2113,8 +2212,12 @@
       <c r="J23" s="2">
         <v>1.4E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="5">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2146,8 +2249,12 @@
       <c r="J24" s="2">
         <v>1.4E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="5">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2179,8 +2286,12 @@
       <c r="J25" s="2">
         <v>1.4E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="5">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2212,8 +2323,12 @@
       <c r="J26" s="2">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2245,8 +2360,12 @@
       <c r="J27" s="2">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2278,8 +2397,12 @@
       <c r="J28" s="2">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2311,8 +2434,12 @@
       <c r="J29" s="2">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2344,8 +2471,12 @@
       <c r="J30" s="2">
         <v>1.4E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K30" s="5">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2377,8 +2508,12 @@
       <c r="J31" s="2">
         <v>5.7000000000000002E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="5">
+        <f t="shared" si="1"/>
+        <v>0.57000000000000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2410,8 +2545,12 @@
       <c r="J32" s="2">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2443,8 +2582,12 @@
       <c r="J33" s="2">
         <v>1.4E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="5">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2476,8 +2619,12 @@
       <c r="J34" s="2">
         <v>1.4E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="5">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2509,8 +2656,12 @@
       <c r="J35" s="2">
         <v>1.2010000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="5">
+        <f t="shared" si="1"/>
+        <v>14.412000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2542,8 +2693,12 @@
       <c r="J36" s="2">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="5">
+        <f t="shared" si="1"/>
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2569,8 +2724,18 @@
         <f t="shared" si="0"/>
         <v>18.45</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
+      <c r="J37" s="2">
+        <v>18.45</v>
+      </c>
+      <c r="K37" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2602,8 +2767,12 @@
       <c r="J38" s="2">
         <v>10.58</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="5">
+        <f t="shared" si="1"/>
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2635,8 +2804,12 @@
       <c r="J39" s="2">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="5">
+        <f t="shared" si="1"/>
+        <v>4.6000000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2668,8 +2841,12 @@
       <c r="J40" s="2">
         <v>0.373</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" s="5">
+        <f t="shared" si="1"/>
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2695,26 +2872,55 @@
         <f t="shared" si="0"/>
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="C42" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="D42" s="1">
         <v>1</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="F42" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G42" s="2">
+        <v>1</v>
+      </c>
       <c r="H42" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1">
+        <v>20</v>
+      </c>
+      <c r="J42" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="K42" s="5">
+        <f t="shared" si="1"/>
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2746,14 +2952,22 @@
       <c r="J43" s="2">
         <v>2.71</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" s="5">
+        <f t="shared" si="1"/>
+        <v>13.55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D44" s="1">
         <v>109</v>
       </c>
       <c r="H44" s="2">
         <f>SUM(H2:H43)</f>
-        <v>62.779999999999994</v>
+        <v>63.779999999999994</v>
+      </c>
+      <c r="K44" s="5">
+        <f>SUM(K2:K43)</f>
+        <v>155.40200000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>